<commit_message>
解决了 UnicodeDecodeError: 'utf-8' codec can't decode
</commit_message>
<xml_diff>
--- a/installRec.xlsx
+++ b/installRec.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="install mysql " sheetId="1" r:id="rId1"/>
     <sheet name="django基本过程" sheetId="2" r:id="rId2"/>
     <sheet name="服务器安装(ubuntu18.04)" sheetId="3" r:id="rId3"/>
+    <sheet name="django问题&amp;解决" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="97">
   <si>
     <t>use mysql</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -700,228 +701,248 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>忘记</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>mysql</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>密码（方法</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>忘记</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>mysql</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>密码（方法</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pip install Django==2.1.7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（降级</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>django</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>查看</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/etc/mysql/debian.cnf</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create user 'test2act'@'localhost' identified by '123';</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update mysql.user set authentication_string=password('123456') where user='root';</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> select host,user from mysql.user;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看数据库用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update mysql.user set authentication_string=password('123') where user='test2act';</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给用户权限（方法1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给用户权限（方法2）</t>
+  </si>
+  <si>
+    <t>source D:\work\site\django\Django_MySQL_Table\ithome_news.sql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mysql -u root -p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pwd654321</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本机配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create database ithome_news;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use ithome_news;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>python3 manage.py runserver 0.0.0.0:8000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">django.core.exceptions.ImproperlyConfigured: mysqlclient 1.3.13 or newer is requ
 ired; you have 0.9.3.
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>忘记</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>mysql</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>密码（方法</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>忘记</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>mysql</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>密码（方法</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>2）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pip install Django==2.1.7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>（降级</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>django</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>查看</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/etc/mysql/debian.cnf</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create user 'test2act'@'localhost' identified by '123';</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>update mysql.user set authentication_string=password('123456') where user='root';</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> select host,user from mysql.user;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看数据库用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>update mysql.user set authentication_string=password('123') where user='test2act';</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>给用户权限（方法1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>给用户权限（方法2）</t>
-  </si>
-  <si>
-    <t>source D:\work\site\django\Django_MySQL_Table\ithome_news.sql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mysql -u root -p</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pwd654321</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本机配置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create database ithome_news;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>use ithome_news;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>python3 manage.py runserver 0.0.0.0:8000</t>
+    <t>N1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UnicodeDecodeError: 'utf-8' codec can't decode byte 0xce in position 254: invalid continuation byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文格式不对。使用UtraEdit修改文字。可能是dreamweave设置问题</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1471,7 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1543,12 +1564,12 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1556,10 +1577,10 @@
     </row>
     <row r="13" spans="1:2" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="20.100000000000001" customHeight="1">
@@ -1572,10 +1593,10 @@
     </row>
     <row r="15" spans="1:2" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.25" customHeight="1">
@@ -1599,30 +1620,30 @@
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
         <v>86</v>
-      </c>
-      <c r="C21" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1684,7 +1705,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -1728,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1862,7 +1883,7 @@
     </row>
     <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
         <v>65</v>
@@ -1870,10 +1891,10 @@
     </row>
     <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1">
@@ -1881,7 +1902,7 @@
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1">
@@ -1911,10 +1932,10 @@
     </row>
     <row r="22" spans="1:3" ht="34.5" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>66</v>
@@ -1931,4 +1952,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="6.75" customWidth="1"/>
+    <col min="2" max="2" width="36.625" customWidth="1"/>
+    <col min="3" max="3" width="24.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="48" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>